<commit_message>
Adding two files from submitted run that were pulled erroneously in test run
</commit_message>
<xml_diff>
--- a/aux/datafiles.xlsx
+++ b/aux/datafiles.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t xml:space="preserve">Order</t>
   </si>
@@ -115,7 +115,13 @@
     <t xml:space="preserve">./data/openalex/affiliation-impute.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">Machine-imputed institutions using auxiliary openAlex information</t>
+  </si>
+  <si>
     <t xml:space="preserve">./data/openalex/affiliations-imputed.Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Records on institutions when available, pulled from openAlex API</t>
   </si>
   <si>
     <t xml:space="preserve">Generated from openAlex data</t>
@@ -160,6 +166,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -219,8 +226,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,15 +244,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -356,357 +358,371 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="43.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="43.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="C19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0" t="s">
+      <c r="A22" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="0" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="0" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="0" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="0" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final edits - all seems to match
- with the exception of a few small numbers related to openAlex
</commit_message>
<xml_diff>
--- a/aux/datafiles.xlsx
+++ b/aux/datafiles.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t xml:space="preserve">Order</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">./data/crossref/crossref_info.Rds</t>
   </si>
   <si>
+    <t xml:space="preserve">./data/crossref/crossref_aejdois.Rds</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hand-generated by authors based on AEA websites</t>
   </si>
   <si>
@@ -134,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">./data/openalex/blacklist.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procedural file to map short names to long variable names</t>
   </si>
   <si>
     <t xml:space="preserve">./data/auxiliary/mainOA-mapping.xlsx</t>
@@ -358,10 +364,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,10 +465,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -470,13 +476,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -487,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -501,7 +507,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -515,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
@@ -529,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
@@ -540,13 +546,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -557,7 +563,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
@@ -568,13 +574,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -585,10 +591,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
@@ -596,13 +602,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
@@ -613,7 +619,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>30</v>
@@ -627,10 +633,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>11</v>
@@ -641,10 +647,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
@@ -658,7 +664,7 @@
         <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
@@ -669,16 +675,22 @@
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
         <v>38</v>
       </c>
@@ -687,16 +699,22 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>6</v>
@@ -704,7 +722,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>6</v>
@@ -712,7 +730,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>6</v>
@@ -720,9 +738,17 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>